<commit_message>
Adding more rows in excel sheet
Adding more rows in excel sheet
</commit_message>
<xml_diff>
--- a/janRain.xlsx
+++ b/janRain.xlsx
@@ -372,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,6 +392,30 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>

</xml_diff>